<commit_message>
dados salvos do codespace
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -462,10 +462,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2458.227157592773</v>
+        <v>71.7768669128418</v>
       </c>
       <c r="C2" t="n">
-        <v>67888</v>
+        <v>96252</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -480,10 +480,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2379.744529724121</v>
+        <v>71.72727584838867</v>
       </c>
       <c r="C3" t="n">
-        <v>75432</v>
+        <v>104700</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -498,10 +498,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2232.174396514893</v>
+        <v>72.11661338806152</v>
       </c>
       <c r="C4" t="n">
-        <v>75880</v>
+        <v>105212</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -516,10 +516,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2226.418018341064</v>
+        <v>73.54855537414551</v>
       </c>
       <c r="C5" t="n">
-        <v>75960</v>
+        <v>105468</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -534,10 +534,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2207.451105117798</v>
+        <v>123.4285831451416</v>
       </c>
       <c r="C6" t="n">
-        <v>76036</v>
+        <v>105596</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -552,10 +552,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2188.704013824463</v>
+        <v>130.6262016296387</v>
       </c>
       <c r="C7" t="n">
-        <v>76040</v>
+        <v>105596</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -570,10 +570,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2189.409255981445</v>
+        <v>71.7930793762207</v>
       </c>
       <c r="C8" t="n">
-        <v>76060</v>
+        <v>105596</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -588,10 +588,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2169.234991073608</v>
+        <v>74.08308982849121</v>
       </c>
       <c r="C9" t="n">
-        <v>76076</v>
+        <v>105596</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -606,10 +606,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2188.690662384033</v>
+        <v>71.31147384643555</v>
       </c>
       <c r="C10" t="n">
-        <v>76080</v>
+        <v>105596</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -624,10 +624,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2139.765501022339</v>
+        <v>92.52834320068359</v>
       </c>
       <c r="C11" t="n">
-        <v>76088</v>
+        <v>105596</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -642,10 +642,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>40467.13757514954</v>
+        <v>15893.02802085876</v>
       </c>
       <c r="C12" t="n">
-        <v>67788</v>
+        <v>95864</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -660,10 +660,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>42052.90246009827</v>
+        <v>11923.79331588745</v>
       </c>
       <c r="C13" t="n">
-        <v>75956</v>
+        <v>105208</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -678,10 +678,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>42206.6638469696</v>
+        <v>11435.37735939026</v>
       </c>
       <c r="C14" t="n">
-        <v>76008</v>
+        <v>105720</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -696,10 +696,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>42407.33051300049</v>
+        <v>11683.5036277771</v>
       </c>
       <c r="C15" t="n">
-        <v>76272</v>
+        <v>105848</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -714,10 +714,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>45395.98417282104</v>
+        <v>13989.67957496643</v>
       </c>
       <c r="C16" t="n">
-        <v>76420</v>
+        <v>105848</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -732,10 +732,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>47876.73902511597</v>
+        <v>15115.25297164917</v>
       </c>
       <c r="C17" t="n">
-        <v>76540</v>
+        <v>105848</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -750,10 +750,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>49578.45497131348</v>
+        <v>11457.23628997803</v>
       </c>
       <c r="C18" t="n">
-        <v>76628</v>
+        <v>105848</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -768,10 +768,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>46294.8944568634</v>
+        <v>11508.92782211304</v>
       </c>
       <c r="C19" t="n">
-        <v>76684</v>
+        <v>105848</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -786,10 +786,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>43860.2569103241</v>
+        <v>11701.92646980286</v>
       </c>
       <c r="C20" t="n">
-        <v>76780</v>
+        <v>105848</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -804,10 +804,10 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>46319.33689117432</v>
+        <v>11540.26675224304</v>
       </c>
       <c r="C21" t="n">
-        <v>76792</v>
+        <v>105848</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>

</xml_diff>